<commit_message>
minor changes to paper
</commit_message>
<xml_diff>
--- a/doc/scorePlot.xlsx
+++ b/doc/scorePlot.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="270" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="135" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -64,7 +64,7 @@
     <t>N=14</t>
   </si>
   <si>
-    <t>With backoff</t>
+    <t>Cumulative</t>
   </si>
 </sst>
 </file>
@@ -99,6 +99,7 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <sz val="13"/>
     </font>
     <font>
@@ -109,6 +110,7 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -243,7 +245,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Baseline Scores</a:t>
             </a:r>
           </a:p>
@@ -730,11 +732,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="69638149"/>
-        <c:axId val="18002779"/>
+        <c:axId val="23277756"/>
+        <c:axId val="15958077"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69638149"/>
+        <c:axId val="23277756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,7 +751,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Threshold</a:t>
                 </a:r>
               </a:p>
@@ -760,8 +762,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="18002779"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="15958077"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -774,7 +776,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18002779"/>
+        <c:axId val="15958077"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,7 +791,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>F1</a:t>
                 </a:r>
               </a:p>
@@ -809,8 +811,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69638149"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="23277756"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -856,7 +858,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>Backoff Scores</a:t>
             </a:r>
           </a:p>
@@ -1818,11 +1820,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="53397967"/>
-        <c:axId val="65859272"/>
+        <c:axId val="34925656"/>
+        <c:axId val="31181151"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53397967"/>
+        <c:axId val="34925656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,7 +1839,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>Threshold</a:t>
                 </a:r>
               </a:p>
@@ -1848,8 +1850,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65859272"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="31181151"/>
+        <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1862,7 +1864,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65859272"/>
+        <c:axId val="31181151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1877,7 +1879,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>F1</a:t>
                 </a:r>
               </a:p>
@@ -1897,8 +1899,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53397967"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="34925656"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -1934,15 +1936,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>770760</xdr:colOff>
+      <xdr:colOff>797760</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>810360</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>16560</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1950,8 +1952,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="770760" y="2651760"/>
-        <a:ext cx="4939920" cy="3153240"/>
+        <a:off x="797760" y="2642760"/>
+        <a:ext cx="4962240" cy="3152880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1968,16 +1970,16 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>108360</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>191160</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>183240</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1985,8 +1987,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5825160" y="1170000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="1011600" y="1910520"/>
+        <a:ext cx="5735520" cy="3351240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2008,12 +2010,12 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="300" zoomScaleNormal="300" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="E12" activeCellId="0" pane="topLeft" sqref="E12"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -2203,7 +2205,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05416666666667" bottom="1.05416666666667" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2219,14 +2221,14 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="H8" view="normal" windowProtection="false" workbookViewId="0" zoomScale="300" zoomScaleNormal="300" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A8" xSplit="0" ySplit="-1"/>
-      <selection activeCell="L33" activeCellId="0" pane="topLeft" sqref="L33"/>
-      <selection activeCell="H8" activeCellId="0" pane="bottomLeft" sqref="H8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B15" view="normal" windowProtection="false" workbookViewId="0" zoomScale="300" zoomScaleNormal="300" zoomScalePageLayoutView="100">
+      <pane activePane="topLeft" topLeftCell="A15" xSplit="0" ySplit="-1"/>
+      <selection activeCell="I16" activeCellId="0" pane="topLeft" sqref="I16"/>
+      <selection activeCell="B15" activeCellId="0" pane="bottomLeft" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -2568,7 +2570,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>